<commit_message>
Updated the activity risk usage.
git-svn-id: https://scrap.dis.anl.gov/repos/MRSA/models/agentmodel@123 eb7698ad-c3c5-4393-a60c-5d690fe7bf3d
</commit_message>
<xml_diff>
--- a/MRSA/data/TransitionMatrix.xlsx
+++ b/MRSA/data/TransitionMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Transition Matrix" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
     <t>For D we assume everyone gets antibiotics that work as follows (Kaplan–Meier Survival Function) (We Will Only Use the Median for Now):</t>
   </si>
   <si>
-    <t>For E we assume everyone gets antibiotics that work as follows (Kaplan–Meier Survival Function) (We Will Only Use the Median for Now):</t>
+    <t>For E we assume spontaneous decolonization (Kaplan–Meier Survival Function) (We Will Only Use the Median for Now):</t>
   </si>
 </sst>
 </file>
@@ -681,30 +681,30 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="77" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="77" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="154">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1191,7 +1191,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1199,21 +1201,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="27" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="27" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="29"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="B2" s="15" t="s">
@@ -1365,43 +1367,43 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -1455,7 +1457,7 @@
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="23"/>
-      <c r="C22" s="33">
+      <c r="C22" s="27">
         <v>0.05</v>
       </c>
       <c r="D22" t="s">
@@ -1469,7 +1471,7 @@
       </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="C23" s="30">
+      <c r="C23" s="24">
         <v>0.5</v>
       </c>
       <c r="D23" t="s">
@@ -1483,7 +1485,7 @@
       </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="C24" s="33">
+      <c r="C24" s="27">
         <v>0.95</v>
       </c>
       <c r="D24" t="s">
@@ -1503,7 +1505,7 @@
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="23"/>
-      <c r="C26" s="33">
+      <c r="C26" s="27">
         <v>0.05</v>
       </c>
       <c r="D26" t="s">
@@ -1517,7 +1519,7 @@
       </c>
     </row>
     <row r="27" spans="2:8">
-      <c r="C27" s="30">
+      <c r="C27" s="24">
         <v>0.5</v>
       </c>
       <c r="D27" t="s">
@@ -1531,7 +1533,7 @@
       </c>
     </row>
     <row r="28" spans="2:8">
-      <c r="C28" s="33">
+      <c r="C28" s="27">
         <v>0.95</v>
       </c>
       <c r="D28" t="s">
@@ -1556,7 +1558,7 @@
       <c r="D31" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="26" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1567,7 +1569,7 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="25">
         <v>0.48799999999999999</v>
       </c>
     </row>
@@ -1578,7 +1580,7 @@
       <c r="D33">
         <v>2</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="25">
         <v>0.28199999999999997</v>
       </c>
     </row>
@@ -1589,7 +1591,7 @@
       <c r="D34">
         <v>3</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="25">
         <v>0.23</v>
       </c>
     </row>
@@ -1600,7 +1602,7 @@
       <c r="D35">
         <v>4</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="25">
         <v>0.21199999999999999</v>
       </c>
     </row>
@@ -1620,7 +1622,6 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Initial optimization of people and activity matching.
git-svn-id: https://scrap.dis.anl.gov/repos/MRSA/models/agentmodel@125 eb7698ad-c3c5-4393-a60c-5d690fe7bf3d
</commit_message>
<xml_diff>
--- a/MRSA/data/TransitionMatrix.xlsx
+++ b/MRSA/data/TransitionMatrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Uncolonized</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>For E we assume spontaneous decolonization (Kaplan–Meier Survival Function) (We Will Only Use the Median for Now):</t>
+  </si>
+  <si>
+    <t>We assume the worst case for exposure in that a person in a place with both C and I people experiences I risk.</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1436,141 +1439,135 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="23" t="s">
-        <v>37</v>
+      <c r="B18" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="22" t="s">
+    <row r="21" spans="2:8">
+      <c r="B21" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="23" t="s">
+    <row r="22" spans="2:8">
+      <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="23"/>
-      <c r="C22" s="27">
+    <row r="23" spans="2:8">
+      <c r="B23" s="23"/>
+      <c r="C23" s="27">
         <v>0.05</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>37</v>
-      </c>
-      <c r="H22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="C23" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23">
-        <v>64</v>
       </c>
       <c r="H23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="C24" s="27">
-        <v>0.95</v>
+      <c r="C24" s="24">
+        <v>0.5</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G24">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="23" t="s">
+      <c r="C25" s="27">
+        <v>0.95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25">
+        <v>91</v>
+      </c>
+      <c r="H25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="23"/>
-      <c r="C26" s="27">
+    <row r="27" spans="2:8">
+      <c r="B27" s="23"/>
+      <c r="C27" s="27">
         <v>0.05</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>38</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>191</v>
-      </c>
-      <c r="H26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="C27" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27">
-        <v>258</v>
       </c>
       <c r="H27" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:8">
-      <c r="C28" s="27">
-        <v>0.95</v>
+      <c r="C28" s="24">
+        <v>0.5</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G28">
-        <v>325</v>
+        <v>258</v>
       </c>
       <c r="H28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
-      <c r="B30" s="23" t="s">
+    <row r="29" spans="2:8">
+      <c r="C29" s="27">
+        <v>0.95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29">
+        <v>325</v>
+      </c>
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="23" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="C31" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="C32" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="25">
-        <v>0.48799999999999999</v>
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="2:5">
@@ -1578,10 +1575,10 @@
         <v>12</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="25">
-        <v>0.28199999999999997</v>
+        <v>0.48799999999999999</v>
       </c>
     </row>
     <row r="34" spans="2:5">
@@ -1589,10 +1586,10 @@
         <v>12</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="25">
-        <v>0.23</v>
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1600,14 +1597,25 @@
         <v>12</v>
       </c>
       <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" s="25">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36">
         <v>4</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E36" s="25">
         <v>0.21199999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="23" t="s">
+    <row r="38" spans="2:5">
+      <c r="B38" s="23" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>